<commit_message>
add compaction performance test
</commit_message>
<xml_diff>
--- a/docs/supportBoolean/boolean compress.xlsx
+++ b/docs/supportBoolean/boolean compress.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>1亿条</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,6 +55,14 @@
   </si>
   <si>
     <t>0.1亿条</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no sort</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sort</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -399,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -557,11 +565,11 @@
         <v>176595</v>
       </c>
       <c r="F9">
-        <f>SUM(D9:E9)</f>
+        <f t="shared" ref="F9:F14" si="0">SUM(D9:E9)</f>
         <v>354621</v>
       </c>
       <c r="G9">
-        <f>C9/F9</f>
+        <f t="shared" ref="G9:G14" si="1">C9/F9</f>
         <v>1691.9188429337237</v>
       </c>
       <c r="I9">
@@ -571,7 +579,7 @@
         <v>99989952</v>
       </c>
       <c r="K9">
-        <f>I9/(J9+I9)</f>
+        <f t="shared" ref="K9:K14" si="2">I9/(J9+I9)</f>
         <v>1.0048E-4</v>
       </c>
     </row>
@@ -589,11 +597,11 @@
         <v>139963</v>
       </c>
       <c r="F10">
-        <f>SUM(D10:E10)</f>
+        <f t="shared" si="0"/>
         <v>281727</v>
       </c>
       <c r="G10">
-        <f>C10/F10</f>
+        <f t="shared" si="1"/>
         <v>2129.7213259644977</v>
       </c>
       <c r="I10">
@@ -603,7 +611,7 @@
         <v>100000000</v>
       </c>
       <c r="K10">
-        <f>I10/(J10+I10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -621,11 +629,11 @@
         <v>139963</v>
       </c>
       <c r="F11">
-        <f>SUM(D11:E11)</f>
+        <f t="shared" si="0"/>
         <v>281727</v>
       </c>
       <c r="G11">
-        <f>C11/F11</f>
+        <f t="shared" si="1"/>
         <v>2129.7213259644977</v>
       </c>
       <c r="I11">
@@ -635,7 +643,7 @@
         <v>100000000</v>
       </c>
       <c r="K11">
-        <f>I11/(J11+I11)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -653,11 +661,11 @@
         <v>139963</v>
       </c>
       <c r="F12">
-        <f>SUM(D12:E12)</f>
+        <f t="shared" si="0"/>
         <v>281727</v>
       </c>
       <c r="G12">
-        <f>C12/F12</f>
+        <f t="shared" si="1"/>
         <v>2129.7213259644977</v>
       </c>
       <c r="I12">
@@ -667,7 +675,7 @@
         <v>100000000</v>
       </c>
       <c r="K12">
-        <f>I12/(J12+I12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -688,11 +696,11 @@
         <v>3572986</v>
       </c>
       <c r="F13">
-        <f>SUM(D13:E13)</f>
+        <f t="shared" si="0"/>
         <v>7211599</v>
       </c>
       <c r="G13">
-        <f>C13/F13</f>
+        <f t="shared" si="1"/>
         <v>83.059250521278287</v>
       </c>
       <c r="I13">
@@ -702,7 +710,7 @@
         <v>98990008</v>
       </c>
       <c r="K13">
-        <f>I13/(J13+I13)</f>
+        <f t="shared" si="2"/>
         <v>1.009992E-2</v>
       </c>
       <c r="M13">
@@ -727,11 +735,11 @@
         <v>3576903</v>
       </c>
       <c r="F14">
-        <f>SUM(D14:E14)</f>
+        <f t="shared" si="0"/>
         <v>7207898</v>
       </c>
       <c r="G14">
-        <f>C14/F14</f>
+        <f t="shared" si="1"/>
         <v>83.10199214805759</v>
       </c>
       <c r="I14">
@@ -741,7 +749,7 @@
         <v>98990683</v>
       </c>
       <c r="K14">
-        <f>I14/(J14+I14)</f>
+        <f t="shared" si="2"/>
         <v>1.009317E-2</v>
       </c>
     </row>
@@ -762,11 +770,11 @@
         <v>3575576</v>
       </c>
       <c r="F15">
-        <f t="shared" ref="F15" si="0">SUM(D15:E15)</f>
+        <f t="shared" ref="F15" si="3">SUM(D15:E15)</f>
         <v>7216120</v>
       </c>
       <c r="G15">
-        <f t="shared" ref="G15" si="1">C15/F15</f>
+        <f t="shared" ref="G15" si="4">C15/F15</f>
         <v>83.007148994196328</v>
       </c>
       <c r="I15">
@@ -776,7 +784,7 @@
         <v>98989548</v>
       </c>
       <c r="K15">
-        <f t="shared" ref="K15:K28" si="2">I15/(J15+I15)</f>
+        <f t="shared" ref="K15:K28" si="5">I15/(J15+I15)</f>
         <v>1.0104520000000001E-2</v>
       </c>
     </row>
@@ -794,11 +802,11 @@
         <v>3546286</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16" si="3">SUM(D16:E16)</f>
+        <f t="shared" ref="F16" si="6">SUM(D16:E16)</f>
         <v>7151813</v>
       </c>
       <c r="G16">
-        <f t="shared" ref="G16" si="4">C16/F16</f>
+        <f t="shared" ref="G16" si="7">C16/F16</f>
         <v>83.754834333615833</v>
       </c>
       <c r="I16">
@@ -808,7 +816,7 @@
         <v>98998913</v>
       </c>
       <c r="K16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.001087E-2</v>
       </c>
     </row>
@@ -826,11 +834,11 @@
         <v>27968080</v>
       </c>
       <c r="F17">
-        <f t="shared" ref="F17:F28" si="5">SUM(D17:E17)</f>
+        <f t="shared" ref="F17:F28" si="8">SUM(D17:E17)</f>
         <v>57286434</v>
       </c>
       <c r="G17">
-        <f t="shared" ref="G17:G28" si="6">C17/F17</f>
+        <f t="shared" ref="G17:G28" si="9">C17/F17</f>
         <v>10.299141765395975</v>
       </c>
       <c r="I17">
@@ -840,7 +848,7 @@
         <v>90001105</v>
       </c>
       <c r="K17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>9.9988949999999993E-2</v>
       </c>
     </row>
@@ -858,11 +866,11 @@
         <v>45172762</v>
       </c>
       <c r="F18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>94230178</v>
       </c>
       <c r="G18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>6.1551997917270196</v>
       </c>
       <c r="I18">
@@ -872,7 +880,7 @@
         <v>80005572</v>
       </c>
       <c r="K18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.19994428</v>
       </c>
     </row>
@@ -890,11 +898,11 @@
         <v>55173346</v>
       </c>
       <c r="F19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>117160245</v>
       </c>
       <c r="G19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4.8651297716217643</v>
       </c>
       <c r="I19">
@@ -904,7 +912,7 @@
         <v>69999796</v>
       </c>
       <c r="K19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.30000204000000003</v>
       </c>
     </row>
@@ -922,11 +930,11 @@
         <v>62166766</v>
       </c>
       <c r="F20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>129672743</v>
       </c>
       <c r="G20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4.3185349522528416</v>
       </c>
       <c r="I20">
@@ -936,7 +944,7 @@
         <v>59996273</v>
       </c>
       <c r="K20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.40003727</v>
       </c>
     </row>
@@ -954,11 +962,11 @@
         <v>65226548</v>
       </c>
       <c r="F21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>133642270</v>
       </c>
       <c r="G21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4.1154178240163084</v>
       </c>
       <c r="I21">
@@ -968,7 +976,7 @@
         <v>49993780</v>
       </c>
       <c r="K21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.50006220000000001</v>
       </c>
     </row>
@@ -1082,11 +1090,11 @@
         <v>65192756</v>
       </c>
       <c r="F25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>129642134</v>
       </c>
       <c r="G25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4.165252694775913</v>
       </c>
       <c r="I25">
@@ -1096,7 +1104,7 @@
         <v>39992248</v>
       </c>
       <c r="K25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.60007752000000003</v>
       </c>
     </row>
@@ -1114,11 +1122,11 @@
         <v>57824274</v>
       </c>
       <c r="F26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>117166621</v>
       </c>
       <c r="G26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4.5234817687539186</v>
       </c>
       <c r="I26">
@@ -1128,7 +1136,7 @@
         <v>30001074</v>
       </c>
       <c r="K26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.69998925999999995</v>
       </c>
     </row>
@@ -1146,11 +1154,11 @@
         <v>45582456</v>
       </c>
       <c r="F27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>94222521</v>
       </c>
       <c r="G27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>5.5189110149154255</v>
       </c>
       <c r="I27">
@@ -1160,7 +1168,7 @@
         <v>20005709</v>
       </c>
       <c r="K27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.79994290999999995</v>
       </c>
     </row>
@@ -1178,11 +1186,11 @@
         <v>27135794</v>
       </c>
       <c r="F28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>57291363</v>
       </c>
       <c r="G28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>8.9018608616450621</v>
       </c>
       <c r="I28">
@@ -1192,7 +1200,7 @@
         <v>9999742</v>
       </c>
       <c r="K28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.90000258</v>
       </c>
     </row>
@@ -1210,11 +1218,11 @@
         <v>132403</v>
       </c>
       <c r="F30">
-        <f t="shared" ref="F30" si="7">SUM(D30:E30)</f>
+        <f t="shared" ref="F30" si="10">SUM(D30:E30)</f>
         <v>281727</v>
       </c>
       <c r="G30">
-        <f t="shared" ref="G30" si="8">C30/F30</f>
+        <f t="shared" ref="G30" si="11">C30/F30</f>
         <v>1774.7677716370813</v>
       </c>
       <c r="I30">
@@ -1224,7 +1232,7 @@
         <v>0</v>
       </c>
       <c r="K30">
-        <f t="shared" ref="K30" si="9">I30/(J30+I30)</f>
+        <f t="shared" ref="K30" si="12">I30/(J30+I30)</f>
         <v>1</v>
       </c>
     </row>
@@ -1242,11 +1250,11 @@
         <v>132403</v>
       </c>
       <c r="F31">
-        <f t="shared" ref="F31" si="10">SUM(D31:E31)</f>
+        <f t="shared" ref="F31" si="13">SUM(D31:E31)</f>
         <v>281727</v>
       </c>
       <c r="G31">
-        <f t="shared" ref="G31" si="11">C31/F31</f>
+        <f t="shared" ref="G31" si="14">C31/F31</f>
         <v>1774.7677716370813</v>
       </c>
       <c r="I31">
@@ -1256,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="K31">
-        <f t="shared" ref="K31:K33" si="12">I31/(J31+I31)</f>
+        <f t="shared" ref="K31:K33" si="15">I31/(J31+I31)</f>
         <v>1</v>
       </c>
     </row>
@@ -1277,11 +1285,11 @@
         <v>1412882</v>
       </c>
       <c r="F32">
-        <f t="shared" ref="F32" si="13">SUM(D32:E32)</f>
+        <f t="shared" ref="F32" si="16">SUM(D32:E32)</f>
         <v>2838776</v>
       </c>
       <c r="G32">
-        <f t="shared" ref="G32" si="14">C32/F32</f>
+        <f t="shared" ref="G32" si="17">C32/F32</f>
         <v>2113.5869825586801</v>
       </c>
       <c r="I32">
@@ -1291,7 +1299,7 @@
         <v>0</v>
       </c>
       <c r="K32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -1309,11 +1317,11 @@
         <v>14323</v>
       </c>
       <c r="F33">
-        <f t="shared" ref="F33" si="15">SUM(D33:E33)</f>
+        <f t="shared" ref="F33" si="18">SUM(D33:E33)</f>
         <v>28646</v>
       </c>
       <c r="G33">
-        <f t="shared" ref="G33" si="16">C33/F33</f>
+        <f t="shared" ref="G33" si="19">C33/F33</f>
         <v>2094.5332681700761</v>
       </c>
       <c r="I33">
@@ -1323,8 +1331,57 @@
         <v>10000000</v>
       </c>
       <c r="K33">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37">
+        <v>0.5</v>
+      </c>
+      <c r="C37">
+        <v>549997283</v>
+      </c>
+      <c r="D37">
+        <v>68409785</v>
+      </c>
+      <c r="E37">
+        <v>65221693</v>
+      </c>
+      <c r="F37">
+        <f t="shared" ref="F37:F38" si="20">SUM(D37:E37)</f>
+        <v>133631478</v>
+      </c>
+      <c r="G37">
+        <f t="shared" ref="G37:G38" si="21">C37/F37</f>
+        <v>4.1157763966361278</v>
+      </c>
+      <c r="K37" t="e">
+        <f t="shared" ref="K37:K38" si="22">I37/(J37+I37)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38">
+        <v>0.5</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="G38" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K38" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>